<commit_message>
Final touches week 2
</commit_message>
<xml_diff>
--- a/Schedule.xlsx
+++ b/Schedule.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/0e0481dd48f7e6bd/Python/52-Weeks-of-Python-and-R-2023/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="75" documentId="11_F25DC773A252ABDACC10487A711C7F6A5BDE58EC" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{D6E06C64-FF8B-475F-BAE5-9F50469C7D5A}"/>
+  <xr:revisionPtr revIDLastSave="80" documentId="11_F25DC773A252ABDACC10487A711C7F6A5BDE58EC" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{48D51514-E29D-423C-985B-6E819F60BF06}"/>
   <bookViews>
     <workbookView xWindow="-28920" yWindow="2925" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="24">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="26">
   <si>
     <t>Week</t>
   </si>
@@ -108,6 +108,12 @@
   </si>
   <si>
     <t>Loans (Data is Plural)</t>
+  </si>
+  <si>
+    <t>Image classification: Cracks in concrete</t>
+  </si>
+  <si>
+    <t>https://www.kaggle.com/code/vishnu0399/ensuring-structural-safety-crack-detection</t>
   </si>
 </sst>
 </file>
@@ -517,7 +523,7 @@
   <dimension ref="A1:E53"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
-      <selection activeCell="C3" sqref="C3"/>
+      <selection activeCell="B5" sqref="B5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -646,14 +652,16 @@
       <c r="D9" s="2"/>
       <c r="E9" s="2"/>
     </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:5" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A10" s="4">
         <v>9</v>
       </c>
       <c r="B10" s="2" t="s">
-        <v>18</v>
-      </c>
-      <c r="C10" s="2"/>
+        <v>24</v>
+      </c>
+      <c r="C10" s="5" t="s">
+        <v>25</v>
+      </c>
       <c r="D10" s="2"/>
       <c r="E10" s="2"/>
     </row>
@@ -662,7 +670,7 @@
         <v>10</v>
       </c>
       <c r="B11" s="2" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="C11" s="2"/>
       <c r="D11" s="2"/>
@@ -673,7 +681,7 @@
         <v>11</v>
       </c>
       <c r="B12" s="2" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="C12" s="2"/>
       <c r="D12" s="2"/>
@@ -684,7 +692,7 @@
         <v>12</v>
       </c>
       <c r="B13" s="2" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="C13" s="2"/>
       <c r="D13" s="2"/>
@@ -694,7 +702,9 @@
       <c r="A14" s="4">
         <v>13</v>
       </c>
-      <c r="B14" s="2"/>
+      <c r="B14" s="2" t="s">
+        <v>22</v>
+      </c>
       <c r="C14" s="2"/>
       <c r="D14" s="2"/>
       <c r="E14" s="2"/>
@@ -1055,11 +1065,12 @@
   </sheetData>
   <hyperlinks>
     <hyperlink ref="C2" r:id="rId1" xr:uid="{BCB2A182-B670-418B-99E0-09A7118C3E4A}"/>
+    <hyperlink ref="C10" r:id="rId2" xr:uid="{8BE852A7-1DA5-49BA-8726-FF07E92CC00C}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId2"/>
+  <pageSetup orientation="portrait" r:id="rId3"/>
   <tableParts count="1">
-    <tablePart r:id="rId3"/>
+    <tablePart r:id="rId4"/>
   </tableParts>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Initial Commit Week 4
</commit_message>
<xml_diff>
--- a/Schedule.xlsx
+++ b/Schedule.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="25831"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="25928"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/0e0481dd48f7e6bd/Python/52-Weeks-of-Python-and-R-2023/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="94" documentId="11_F25DC773A252ABDACC10487A711C7F6A5BDE58EC" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{12535C37-AF23-42B8-8BCF-51ABAF535263}"/>
+  <xr:revisionPtr revIDLastSave="99" documentId="11_F25DC773A252ABDACC10487A711C7F6A5BDE58EC" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{D05A9C8B-5D1D-4D27-8D21-D5986897B773}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="25820" windowHeight="15500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-28920" yWindow="2925" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="31" uniqueCount="31">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="33" uniqueCount="33">
   <si>
     <t>Week</t>
   </si>
@@ -129,6 +129,12 @@
   </si>
   <si>
     <t>Luxembourg Stats (Compare weather with St. Gallen?)</t>
+  </si>
+  <si>
+    <t>Scraping and visualising housing prices for different post codes in Vienna</t>
+  </si>
+  <si>
+    <t>Lookback on the Gym Year (Gym Tracking)</t>
   </si>
 </sst>
 </file>
@@ -537,8 +543,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:E53"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A8" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
-      <selection activeCell="B16" sqref="B16"/>
+    <sheetView showGridLines="0" tabSelected="1" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
+      <selection activeCell="B53" sqref="B53"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -640,12 +646,12 @@
       <c r="D6" s="2"/>
       <c r="E6" s="2"/>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:5" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A7" s="4">
         <v>6</v>
       </c>
       <c r="B7" s="2" t="s">
-        <v>14</v>
+        <v>31</v>
       </c>
       <c r="C7" s="2"/>
       <c r="D7" s="2"/>
@@ -656,18 +662,18 @@
         <v>7</v>
       </c>
       <c r="B8" s="2" t="s">
-        <v>22</v>
+        <v>14</v>
       </c>
       <c r="C8" s="2"/>
       <c r="D8" s="2"/>
       <c r="E8" s="2"/>
     </row>
-    <row r="9" spans="1:5" ht="43.5" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A9" s="4">
         <v>8</v>
       </c>
       <c r="B9" s="2" t="s">
-        <v>20</v>
+        <v>22</v>
       </c>
       <c r="C9" s="2"/>
       <c r="D9" s="2"/>
@@ -678,22 +684,22 @@
         <v>9</v>
       </c>
       <c r="B10" s="2" t="s">
-        <v>23</v>
-      </c>
-      <c r="C10" s="5" t="s">
-        <v>24</v>
-      </c>
+        <v>20</v>
+      </c>
+      <c r="C10" s="2"/>
       <c r="D10" s="2"/>
       <c r="E10" s="2"/>
     </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:5" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A11" s="4">
         <v>10</v>
       </c>
       <c r="B11" s="2" t="s">
-        <v>18</v>
-      </c>
-      <c r="C11" s="2"/>
+        <v>23</v>
+      </c>
+      <c r="C11" s="5" t="s">
+        <v>24</v>
+      </c>
       <c r="D11" s="2"/>
       <c r="E11" s="2"/>
     </row>
@@ -702,7 +708,7 @@
         <v>11</v>
       </c>
       <c r="B12" s="2" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="C12" s="2"/>
       <c r="D12" s="2"/>
@@ -713,50 +719,52 @@
         <v>12</v>
       </c>
       <c r="B13" s="2" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="C13" s="2"/>
       <c r="D13" s="2"/>
       <c r="E13" s="2"/>
     </row>
-    <row r="14" spans="1:5" ht="58" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A14" s="4">
         <v>13</v>
       </c>
       <c r="B14" s="2" t="s">
-        <v>25</v>
+        <v>21</v>
       </c>
       <c r="C14" s="2"/>
       <c r="D14" s="2"/>
       <c r="E14" s="2"/>
     </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:5" ht="58" x14ac:dyDescent="0.35">
       <c r="A15" s="4">
         <v>14</v>
       </c>
       <c r="B15" s="2" t="s">
-        <v>29</v>
+        <v>25</v>
       </c>
       <c r="C15" s="2"/>
       <c r="D15" s="2"/>
       <c r="E15" s="2"/>
     </row>
-    <row r="16" spans="1:5" ht="29" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A16" s="4">
         <v>15</v>
       </c>
       <c r="B16" s="2" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="C16" s="2"/>
       <c r="D16" s="2"/>
       <c r="E16" s="2"/>
     </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:5" ht="29" x14ac:dyDescent="0.35">
       <c r="A17" s="4">
         <v>16</v>
       </c>
-      <c r="B17" s="2"/>
+      <c r="B17" s="2" t="s">
+        <v>30</v>
+      </c>
       <c r="C17" s="2"/>
       <c r="D17" s="2"/>
       <c r="E17" s="2"/>
@@ -1069,11 +1077,13 @@
       <c r="D51" s="2"/>
       <c r="E51" s="2"/>
     </row>
-    <row r="52" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="52" spans="1:5" ht="29" x14ac:dyDescent="0.35">
       <c r="A52" s="4">
         <v>51</v>
       </c>
-      <c r="B52" s="2"/>
+      <c r="B52" s="2" t="s">
+        <v>32</v>
+      </c>
       <c r="C52" s="2"/>
       <c r="D52" s="2"/>
       <c r="E52" s="2"/>
@@ -1090,7 +1100,7 @@
   </sheetData>
   <hyperlinks>
     <hyperlink ref="C2" r:id="rId1" xr:uid="{BCB2A182-B670-418B-99E0-09A7118C3E4A}"/>
-    <hyperlink ref="C10" r:id="rId2" xr:uid="{8BE852A7-1DA5-49BA-8726-FF07E92CC00C}"/>
+    <hyperlink ref="C11" r:id="rId2" xr:uid="{8BE852A7-1DA5-49BA-8726-FF07E92CC00C}"/>
     <hyperlink ref="C5" r:id="rId3" xr:uid="{9AA2BF18-F5AA-42E4-B5EA-240371BBCC34}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Week 5 final commit
</commit_message>
<xml_diff>
--- a/Schedule.xlsx
+++ b/Schedule.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="25928"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26026"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/0e0481dd48f7e6bd/Python/52-Weeks-of-Python-and-R-2023/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="99" documentId="11_F25DC773A252ABDACC10487A711C7F6A5BDE58EC" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{D05A9C8B-5D1D-4D27-8D21-D5986897B773}"/>
+  <xr:revisionPtr revIDLastSave="133" documentId="11_F25DC773A252ABDACC10487A711C7F6A5BDE58EC" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{B7B2E513-F1E7-4911-A7CE-D30E3DE28705}"/>
   <bookViews>
-    <workbookView xWindow="-28920" yWindow="2925" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="25820" windowHeight="15500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="33" uniqueCount="33">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="42" uniqueCount="42">
   <si>
     <t>Week</t>
   </si>
@@ -80,9 +80,6 @@
     <t>Get visual insights from the data</t>
   </si>
   <si>
-    <t>Predicting the price of used cars</t>
-  </si>
-  <si>
     <t>Unisport Bern Occupancy</t>
   </si>
   <si>
@@ -131,10 +128,40 @@
     <t>Luxembourg Stats (Compare weather with St. Gallen?)</t>
   </si>
   <si>
-    <t>Scraping and visualising housing prices for different post codes in Vienna</t>
-  </si>
-  <si>
     <t>Lookback on the Gym Year (Gym Tracking)</t>
+  </si>
+  <si>
+    <t>World Bank Data?</t>
+  </si>
+  <si>
+    <t>Scrape rent prices for all of Brussels from the website of a major Belgian real estate platform. Then clean, visualise and model these data.</t>
+  </si>
+  <si>
+    <t>Web Scraping, Selenium, RSelenium, ggplot2, dplyr, pandas, seaborn, matplotlib, Feature Selection, Data Cleaning, Regression Models</t>
+  </si>
+  <si>
+    <t>https://www.immoweb.be/en/search/house-and-apartment/for-rent/brussels/province?countries=BE&amp;page=1&amp;orderBy=newest</t>
+  </si>
+  <si>
+    <t>Scraping and visualising housing prices for different post codes in Vienna, including descriptions</t>
+  </si>
+  <si>
+    <t>Predicting used car prices</t>
+  </si>
+  <si>
+    <t>Brussels Rent Prices Webscraping Selenium + Modelling</t>
+  </si>
+  <si>
+    <t>Bern Rent Prices vs. Vienna vs. Brussels vs. London vs. New York</t>
+  </si>
+  <si>
+    <t>New York Open Data</t>
+  </si>
+  <si>
+    <t>https://data.cityofnewyork.us/browse?category=Health</t>
+  </si>
+  <si>
+    <t>Scraping Rolex Prices</t>
   </si>
 </sst>
 </file>
@@ -543,8 +570,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:E53"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
-      <selection activeCell="B53" sqref="B53"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A10" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
+      <selection activeCell="C22" sqref="C22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -614,10 +641,10 @@
       </c>
       <c r="C4" s="2"/>
       <c r="D4" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="E4" s="2" t="s">
         <v>27</v>
-      </c>
-      <c r="E4" s="2" t="s">
-        <v>28</v>
       </c>
     </row>
     <row r="5" spans="1:5" ht="58" x14ac:dyDescent="0.35">
@@ -628,30 +655,36 @@
         <v>11</v>
       </c>
       <c r="C5" s="5" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="D5" s="2" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="E5" s="2"/>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:5" ht="72.5" x14ac:dyDescent="0.35">
       <c r="A6" s="4">
         <v>5</v>
       </c>
       <c r="B6" s="2" t="s">
-        <v>17</v>
-      </c>
-      <c r="C6" s="2"/>
-      <c r="D6" s="2"/>
-      <c r="E6" s="2"/>
+        <v>37</v>
+      </c>
+      <c r="C6" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="D6" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="E6" s="2" t="s">
+        <v>33</v>
+      </c>
     </row>
     <row r="7" spans="1:5" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A7" s="4">
         <v>6</v>
       </c>
       <c r="B7" s="2" t="s">
-        <v>31</v>
+        <v>35</v>
       </c>
       <c r="C7" s="2"/>
       <c r="D7" s="2"/>
@@ -662,7 +695,7 @@
         <v>7</v>
       </c>
       <c r="B8" s="2" t="s">
-        <v>14</v>
+        <v>36</v>
       </c>
       <c r="C8" s="2"/>
       <c r="D8" s="2"/>
@@ -673,7 +706,7 @@
         <v>8</v>
       </c>
       <c r="B9" s="2" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="C9" s="2"/>
       <c r="D9" s="2"/>
@@ -684,7 +717,7 @@
         <v>9</v>
       </c>
       <c r="B10" s="2" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="C10" s="2"/>
       <c r="D10" s="2"/>
@@ -695,10 +728,10 @@
         <v>10</v>
       </c>
       <c r="B11" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="C11" s="5" t="s">
         <v>23</v>
-      </c>
-      <c r="C11" s="5" t="s">
-        <v>24</v>
       </c>
       <c r="D11" s="2"/>
       <c r="E11" s="2"/>
@@ -708,7 +741,7 @@
         <v>11</v>
       </c>
       <c r="B12" s="2" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="C12" s="2"/>
       <c r="D12" s="2"/>
@@ -719,7 +752,7 @@
         <v>12</v>
       </c>
       <c r="B13" s="2" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="C13" s="2"/>
       <c r="D13" s="2"/>
@@ -730,7 +763,7 @@
         <v>13</v>
       </c>
       <c r="B14" s="2" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="C14" s="2"/>
       <c r="D14" s="2"/>
@@ -741,7 +774,7 @@
         <v>14</v>
       </c>
       <c r="B15" s="2" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="C15" s="2"/>
       <c r="D15" s="2"/>
@@ -752,7 +785,7 @@
         <v>15</v>
       </c>
       <c r="B16" s="2" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="C16" s="2"/>
       <c r="D16" s="2"/>
@@ -763,7 +796,7 @@
         <v>16</v>
       </c>
       <c r="B17" s="2" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="C17" s="2"/>
       <c r="D17" s="2"/>
@@ -773,7 +806,9 @@
       <c r="A18" s="4">
         <v>17</v>
       </c>
-      <c r="B18" s="2"/>
+      <c r="B18" s="2" t="s">
+        <v>16</v>
+      </c>
       <c r="C18" s="2"/>
       <c r="D18" s="2"/>
       <c r="E18" s="2"/>
@@ -782,16 +817,20 @@
       <c r="A19" s="4">
         <v>18</v>
       </c>
-      <c r="B19" s="2"/>
+      <c r="B19" s="2" t="s">
+        <v>31</v>
+      </c>
       <c r="C19" s="2"/>
       <c r="D19" s="2"/>
       <c r="E19" s="2"/>
     </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:5" ht="29" x14ac:dyDescent="0.35">
       <c r="A20" s="4">
         <v>19</v>
       </c>
-      <c r="B20" s="2"/>
+      <c r="B20" s="2" t="s">
+        <v>38</v>
+      </c>
       <c r="C20" s="2"/>
       <c r="D20" s="2"/>
       <c r="E20" s="2"/>
@@ -800,8 +839,12 @@
       <c r="A21" s="4">
         <v>20</v>
       </c>
-      <c r="B21" s="2"/>
-      <c r="C21" s="2"/>
+      <c r="B21" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="C21" s="2" t="s">
+        <v>40</v>
+      </c>
       <c r="D21" s="2"/>
       <c r="E21" s="2"/>
     </row>
@@ -809,7 +852,9 @@
       <c r="A22" s="4">
         <v>21</v>
       </c>
-      <c r="B22" s="2"/>
+      <c r="B22" s="2" t="s">
+        <v>41</v>
+      </c>
       <c r="C22" s="2"/>
       <c r="D22" s="2"/>
       <c r="E22" s="2"/>
@@ -1053,7 +1098,7 @@
         <v>48</v>
       </c>
       <c r="B49" s="2" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="C49" s="2"/>
       <c r="D49" s="2"/>
@@ -1082,7 +1127,7 @@
         <v>51</v>
       </c>
       <c r="B52" s="2" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="C52" s="2"/>
       <c r="D52" s="2"/>

</xml_diff>

<commit_message>
Week 9 initial commit
</commit_message>
<xml_diff>
--- a/Schedule.xlsx
+++ b/Schedule.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26026"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26130"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/0e0481dd48f7e6bd/Python/52-Weeks-of-Python-and-R-2023/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="161" documentId="11_F25DC773A252ABDACC10487A711C7F6A5BDE58EC" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{DFF6E32B-FA4F-4ED1-8B7B-EA81A2AF715A}"/>
+  <xr:revisionPtr revIDLastSave="167" documentId="11_F25DC773A252ABDACC10487A711C7F6A5BDE58EC" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{CDBCD9A3-1857-4704-9DFF-397A8A9D193A}"/>
   <bookViews>
-    <workbookView xWindow="38235" yWindow="3750" windowWidth="29130" windowHeight="15810" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="38280" yWindow="3795" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="48" uniqueCount="48">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="50" uniqueCount="50">
   <si>
     <t>Week</t>
   </si>
@@ -89,12 +89,6 @@
     <t>Replicate David Robinson Video</t>
   </si>
   <si>
-    <t>Electricity something</t>
-  </si>
-  <si>
-    <t>Prisoners problem</t>
-  </si>
-  <si>
     <t>Procrastinated one about importance of retraining model (Day ahead spot prices)</t>
   </si>
   <si>
@@ -180,6 +174,18 @@
   </si>
   <si>
     <t>Reinforcement Learning Project</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Fear and Greed </t>
+  </si>
+  <si>
+    <t>https://edition.cnn.com/markets/fear-and-greed</t>
+  </si>
+  <si>
+    <t>Check if PE ratio cycles exist and if they have predictive power for long term stock price cycles, like overbought and oversold, try that as well</t>
+  </si>
+  <si>
+    <t>SQL</t>
   </si>
 </sst>
 </file>
@@ -232,7 +238,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
@@ -249,6 +255,7 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -584,8 +591,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:E53"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A9" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
-      <selection activeCell="C12" sqref="C12"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A10" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
+      <selection activeCell="B16" sqref="B16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -655,10 +662,10 @@
       </c>
       <c r="C4" s="2"/>
       <c r="D4" s="2" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="E4" s="2" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
     </row>
     <row r="5" spans="1:5" ht="58" x14ac:dyDescent="0.35">
@@ -669,7 +676,7 @@
         <v>11</v>
       </c>
       <c r="C5" s="5" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="D5" s="2" t="s">
         <v>15</v>
@@ -681,16 +688,16 @@
         <v>5</v>
       </c>
       <c r="B6" s="2" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="C6" s="2" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="D6" s="2" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="E6" s="2" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
     </row>
     <row r="7" spans="1:5" ht="43.5" x14ac:dyDescent="0.35">
@@ -698,10 +705,10 @@
         <v>6</v>
       </c>
       <c r="B7" s="2" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="C7" s="2" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="D7" s="2"/>
       <c r="E7" s="2"/>
@@ -711,10 +718,10 @@
         <v>7</v>
       </c>
       <c r="B8" s="2" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="C8" s="2" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="D8" s="2"/>
       <c r="E8" s="2"/>
@@ -724,11 +731,11 @@
         <v>8</v>
       </c>
       <c r="B9" s="2" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="C9" s="2"/>
       <c r="D9" s="2" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="E9" s="2"/>
     </row>
@@ -737,7 +744,7 @@
         <v>9</v>
       </c>
       <c r="B10" s="2" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="C10" s="2"/>
       <c r="D10" s="2"/>
@@ -748,7 +755,7 @@
         <v>10</v>
       </c>
       <c r="B11" s="2" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="C11" s="5"/>
       <c r="D11" s="2"/>
@@ -759,7 +766,7 @@
         <v>11</v>
       </c>
       <c r="B12" s="2" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="C12" s="2"/>
       <c r="D12" s="2"/>
@@ -770,33 +777,35 @@
         <v>12</v>
       </c>
       <c r="B13" s="2" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="C13" s="2"/>
       <c r="D13" s="2"/>
       <c r="E13" s="2"/>
     </row>
-    <row r="14" spans="1:5" ht="43.5" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A14" s="4">
         <v>13</v>
       </c>
       <c r="B14" s="2" t="s">
-        <v>22</v>
-      </c>
-      <c r="C14" s="2" t="s">
-        <v>23</v>
+        <v>46</v>
+      </c>
+      <c r="C14" s="6" t="s">
+        <v>47</v>
       </c>
       <c r="D14" s="2"/>
       <c r="E14" s="2"/>
     </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:5" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A15" s="4">
         <v>14</v>
       </c>
       <c r="B15" s="2" t="s">
-        <v>17</v>
-      </c>
-      <c r="C15" s="2"/>
+        <v>20</v>
+      </c>
+      <c r="C15" s="2" t="s">
+        <v>21</v>
+      </c>
       <c r="D15" s="2"/>
       <c r="E15" s="2"/>
     </row>
@@ -805,51 +814,51 @@
         <v>15</v>
       </c>
       <c r="B16" s="2" t="s">
-        <v>18</v>
+        <v>49</v>
       </c>
       <c r="C16" s="2"/>
       <c r="D16" s="2"/>
       <c r="E16" s="2"/>
     </row>
-    <row r="17" spans="1:5" ht="58" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:5" ht="72.5" x14ac:dyDescent="0.35">
       <c r="A17" s="4">
         <v>16</v>
       </c>
       <c r="B17" s="2" t="s">
-        <v>24</v>
+        <v>48</v>
       </c>
       <c r="C17" s="2"/>
       <c r="D17" s="2"/>
       <c r="E17" s="2"/>
     </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:5" ht="58" x14ac:dyDescent="0.35">
       <c r="A18" s="4">
         <v>17</v>
       </c>
       <c r="B18" s="2" t="s">
-        <v>28</v>
+        <v>22</v>
       </c>
       <c r="C18" s="2"/>
       <c r="D18" s="2"/>
       <c r="E18" s="2"/>
     </row>
-    <row r="19" spans="1:5" ht="29" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A19" s="4">
         <v>18</v>
       </c>
       <c r="B19" s="2" t="s">
-        <v>29</v>
+        <v>26</v>
       </c>
       <c r="C19" s="2"/>
       <c r="D19" s="2"/>
       <c r="E19" s="2"/>
     </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:5" ht="29" x14ac:dyDescent="0.35">
       <c r="A20" s="4">
         <v>19</v>
       </c>
       <c r="B20" s="2" t="s">
-        <v>16</v>
+        <v>27</v>
       </c>
       <c r="C20" s="2"/>
       <c r="D20" s="2"/>
@@ -860,29 +869,29 @@
         <v>20</v>
       </c>
       <c r="B21" s="2" t="s">
-        <v>31</v>
+        <v>16</v>
       </c>
       <c r="C21" s="2"/>
       <c r="D21" s="2"/>
       <c r="E21" s="2"/>
     </row>
-    <row r="22" spans="1:5" ht="29" x14ac:dyDescent="0.35">
+    <row r="22" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A22" s="4">
         <v>21</v>
       </c>
       <c r="B22" s="2" t="s">
-        <v>35</v>
+        <v>29</v>
       </c>
       <c r="C22" s="2"/>
       <c r="D22" s="2"/>
       <c r="E22" s="2"/>
     </row>
-    <row r="23" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="23" spans="1:5" ht="29" x14ac:dyDescent="0.35">
       <c r="A23" s="4">
         <v>22</v>
       </c>
       <c r="B23" s="2" t="s">
-        <v>39</v>
+        <v>33</v>
       </c>
       <c r="C23" s="2"/>
       <c r="D23" s="2"/>
@@ -893,7 +902,7 @@
         <v>23</v>
       </c>
       <c r="B24" s="2" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
       <c r="C24" s="2"/>
       <c r="D24" s="2"/>
@@ -904,7 +913,7 @@
         <v>24</v>
       </c>
       <c r="B25" s="2" t="s">
-        <v>41</v>
+        <v>38</v>
       </c>
       <c r="C25" s="2"/>
       <c r="D25" s="2"/>
@@ -915,7 +924,7 @@
         <v>25</v>
       </c>
       <c r="B26" s="2" t="s">
-        <v>21</v>
+        <v>39</v>
       </c>
       <c r="C26" s="2"/>
       <c r="D26" s="2"/>
@@ -925,7 +934,9 @@
       <c r="A27" s="4">
         <v>26</v>
       </c>
-      <c r="B27" s="2"/>
+      <c r="B27" s="2" t="s">
+        <v>19</v>
+      </c>
       <c r="C27" s="2"/>
       <c r="D27" s="2"/>
       <c r="E27" s="2"/>
@@ -1153,7 +1164,7 @@
         <v>51</v>
       </c>
       <c r="B52" s="2" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="C52" s="2"/>
       <c r="D52" s="2"/>
@@ -1172,11 +1183,12 @@
   <hyperlinks>
     <hyperlink ref="C2" r:id="rId1" xr:uid="{BCB2A182-B670-418B-99E0-09A7118C3E4A}"/>
     <hyperlink ref="C5" r:id="rId2" xr:uid="{9AA2BF18-F5AA-42E4-B5EA-240371BBCC34}"/>
+    <hyperlink ref="C14" r:id="rId3" xr:uid="{26F759F8-BC11-420B-9F21-9D0D36433723}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId3"/>
+  <pageSetup orientation="portrait" r:id="rId4"/>
   <tableParts count="1">
-    <tablePart r:id="rId4"/>
+    <tablePart r:id="rId5"/>
   </tableParts>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Week 11 final commit
</commit_message>
<xml_diff>
--- a/Schedule.xlsx
+++ b/Schedule.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/0e0481dd48f7e6bd/Python/52-Weeks-of-Python-and-R-2023/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="182" documentId="11_F25DC773A252ABDACC10487A711C7F6A5BDE58EC" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{52CCDAE0-61A4-41CF-BD89-BAE0A8ED5CCC}"/>
+  <xr:revisionPtr revIDLastSave="184" documentId="11_F25DC773A252ABDACC10487A711C7F6A5BDE58EC" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{9B0A6D70-0C02-47F0-A4F3-85F85BB16189}"/>
   <bookViews>
     <workbookView xWindow="38280" yWindow="3795" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="55" uniqueCount="55">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="56" uniqueCount="56">
   <si>
     <t>Week</t>
   </si>
@@ -201,6 +201,9 @@
   </si>
   <si>
     <t>Learn how tune the hyperparameters of a Neural Network in Pytorch Lightning</t>
+  </si>
+  <si>
+    <t>Optuna for Hyperparameter Optimisation</t>
   </si>
 </sst>
 </file>
@@ -605,8 +608,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:E53"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A9" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
-      <selection activeCell="C14" sqref="C14"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A17" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
+      <selection activeCell="B29" sqref="B29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -965,11 +968,13 @@
       <c r="D27" s="2"/>
       <c r="E27" s="2"/>
     </row>
-    <row r="28" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="28" spans="1:5" ht="29" x14ac:dyDescent="0.35">
       <c r="A28" s="4">
         <v>27</v>
       </c>
-      <c r="B28" s="2"/>
+      <c r="B28" s="2" t="s">
+        <v>55</v>
+      </c>
       <c r="C28" s="2"/>
       <c r="D28" s="2"/>
       <c r="E28" s="2"/>

</xml_diff>

<commit_message>
Week 15 and 16
</commit_message>
<xml_diff>
--- a/Schedule.xlsx
+++ b/Schedule.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26130"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26327"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/0e0481dd48f7e6bd/Python/52-Weeks-of-Python-and-R-2023/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="185" documentId="11_F25DC773A252ABDACC10487A711C7F6A5BDE58EC" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{2FFABB38-276A-4F88-894C-A2BF7CCA3D4C}"/>
+  <xr:revisionPtr revIDLastSave="209" documentId="11_F25DC773A252ABDACC10487A711C7F6A5BDE58EC" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{7627A48F-DA44-46B9-84C6-307534C37801}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="25820" windowHeight="15500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="38280" yWindow="3795" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="57" uniqueCount="57">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="64" uniqueCount="64">
   <si>
     <t>Week</t>
   </si>
@@ -122,9 +122,6 @@
     <t>Luxembourg Stats (Compare weather with St. Gallen?)</t>
   </si>
   <si>
-    <t>Lookback on the Gym Year (Gym Tracking)</t>
-  </si>
-  <si>
     <t>World Bank Data?</t>
   </si>
   <si>
@@ -207,6 +204,30 @@
   </si>
   <si>
     <t>Motorcycle Web Scraping</t>
+  </si>
+  <si>
+    <t>Lookback on the year</t>
+  </si>
+  <si>
+    <t>Easter Weather</t>
+  </si>
+  <si>
+    <t>Cartpole Cross Entropy Method</t>
+  </si>
+  <si>
+    <t>FrozenLake Value Iteration</t>
+  </si>
+  <si>
+    <t>LSTM/RNN for Time Series Data</t>
+  </si>
+  <si>
+    <t>FrozenLake Tabular Q-Learning</t>
+  </si>
+  <si>
+    <t>Moonlander Deep Q-Networks</t>
+  </si>
+  <si>
+    <t>Cartpole Advantage Actor Critic</t>
   </si>
 </sst>
 </file>
@@ -611,8 +632,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:E53"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A23" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
-      <selection activeCell="B30" sqref="B30"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A10" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
+      <selection activeCell="B20" sqref="B20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -708,16 +729,16 @@
         <v>5</v>
       </c>
       <c r="B6" s="2" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="C6" s="2" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="D6" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="E6" s="2" t="s">
         <v>30</v>
-      </c>
-      <c r="E6" s="2" t="s">
-        <v>31</v>
       </c>
     </row>
     <row r="7" spans="1:5" ht="43.5" x14ac:dyDescent="0.35">
@@ -725,10 +746,10 @@
         <v>6</v>
       </c>
       <c r="B7" s="2" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="C7" s="2" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="D7" s="2"/>
       <c r="E7" s="2"/>
@@ -738,10 +759,10 @@
         <v>7</v>
       </c>
       <c r="B8" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="C8" s="2" t="s">
         <v>34</v>
-      </c>
-      <c r="C8" s="2" t="s">
-        <v>35</v>
       </c>
       <c r="D8" s="2"/>
       <c r="E8" s="2"/>
@@ -751,11 +772,11 @@
         <v>8</v>
       </c>
       <c r="B9" s="2" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="C9" s="2"/>
       <c r="D9" s="2" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="E9" s="2"/>
     </row>
@@ -768,7 +789,7 @@
       </c>
       <c r="C10" s="2"/>
       <c r="D10" s="2" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="E10" s="2"/>
     </row>
@@ -781,7 +802,7 @@
       </c>
       <c r="C11" s="5"/>
       <c r="D11" s="2" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="E11" s="2"/>
     </row>
@@ -790,11 +811,11 @@
         <v>11</v>
       </c>
       <c r="B12" s="2" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="C12" s="2"/>
       <c r="D12" s="2" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="E12" s="2"/>
     </row>
@@ -803,39 +824,33 @@
         <v>12</v>
       </c>
       <c r="B13" s="2" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="C13" s="2"/>
       <c r="D13" s="2" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="E13" s="2"/>
     </row>
-    <row r="14" spans="1:5" ht="43.5" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A14" s="4">
         <v>13</v>
       </c>
       <c r="B14" s="2" t="s">
-        <v>20</v>
-      </c>
-      <c r="C14" s="2" t="s">
-        <v>21</v>
-      </c>
-      <c r="D14" s="2" t="s">
-        <v>51</v>
-      </c>
+        <v>57</v>
+      </c>
+      <c r="C14" s="2"/>
+      <c r="D14" s="2"/>
       <c r="E14" s="2"/>
     </row>
-    <row r="15" spans="1:5" ht="29" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A15" s="4">
         <v>14</v>
       </c>
       <c r="B15" s="2" t="s">
-        <v>44</v>
-      </c>
-      <c r="C15" s="5" t="s">
-        <v>45</v>
-      </c>
+        <v>58</v>
+      </c>
+      <c r="C15" s="2"/>
       <c r="D15" s="2"/>
       <c r="E15" s="2"/>
     </row>
@@ -844,29 +859,29 @@
         <v>15</v>
       </c>
       <c r="B16" s="2" t="s">
-        <v>47</v>
+        <v>59</v>
       </c>
       <c r="C16" s="2"/>
       <c r="D16" s="2"/>
       <c r="E16" s="2"/>
     </row>
-    <row r="17" spans="1:5" ht="72.5" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A17" s="4">
         <v>16</v>
       </c>
       <c r="B17" s="2" t="s">
-        <v>46</v>
+        <v>61</v>
       </c>
       <c r="C17" s="2"/>
       <c r="D17" s="2"/>
       <c r="E17" s="2"/>
     </row>
-    <row r="18" spans="1:5" ht="58" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A18" s="4">
         <v>17</v>
       </c>
       <c r="B18" s="2" t="s">
-        <v>22</v>
+        <v>62</v>
       </c>
       <c r="C18" s="2"/>
       <c r="D18" s="2"/>
@@ -877,19 +892,17 @@
         <v>18</v>
       </c>
       <c r="B19" s="2" t="s">
-        <v>26</v>
+        <v>63</v>
       </c>
       <c r="C19" s="2"/>
       <c r="D19" s="2"/>
       <c r="E19" s="2"/>
     </row>
-    <row r="20" spans="1:5" ht="29" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A20" s="4">
         <v>19</v>
       </c>
-      <c r="B20" s="2" t="s">
-        <v>27</v>
-      </c>
+      <c r="B20" s="2"/>
       <c r="C20" s="2"/>
       <c r="D20" s="2"/>
       <c r="E20" s="2"/>
@@ -898,9 +911,7 @@
       <c r="A21" s="4">
         <v>20</v>
       </c>
-      <c r="B21" s="2" t="s">
-        <v>16</v>
-      </c>
+      <c r="B21" s="2"/>
       <c r="C21" s="2"/>
       <c r="D21" s="2"/>
       <c r="E21" s="2"/>
@@ -909,32 +920,32 @@
       <c r="A22" s="4">
         <v>21</v>
       </c>
-      <c r="B22" s="2" t="s">
-        <v>29</v>
-      </c>
+      <c r="B22" s="2"/>
       <c r="C22" s="2"/>
       <c r="D22" s="2"/>
       <c r="E22" s="2"/>
     </row>
-    <row r="23" spans="1:5" ht="29" x14ac:dyDescent="0.35">
+    <row r="23" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A23" s="4">
         <v>22</v>
       </c>
       <c r="B23" s="2" t="s">
-        <v>33</v>
+        <v>60</v>
       </c>
       <c r="C23" s="2"/>
       <c r="D23" s="2"/>
       <c r="E23" s="2"/>
     </row>
-    <row r="24" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="24" spans="1:5" ht="29" x14ac:dyDescent="0.35">
       <c r="A24" s="4">
         <v>23</v>
       </c>
       <c r="B24" s="2" t="s">
-        <v>37</v>
-      </c>
-      <c r="C24" s="2"/>
+        <v>43</v>
+      </c>
+      <c r="C24" s="5" t="s">
+        <v>44</v>
+      </c>
       <c r="D24" s="2"/>
       <c r="E24" s="2"/>
     </row>
@@ -943,51 +954,51 @@
         <v>24</v>
       </c>
       <c r="B25" s="2" t="s">
-        <v>38</v>
+        <v>46</v>
       </c>
       <c r="C25" s="2"/>
       <c r="D25" s="2"/>
       <c r="E25" s="2"/>
     </row>
-    <row r="26" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="26" spans="1:5" ht="72.5" x14ac:dyDescent="0.35">
       <c r="A26" s="4">
         <v>25</v>
       </c>
       <c r="B26" s="2" t="s">
-        <v>39</v>
+        <v>45</v>
       </c>
       <c r="C26" s="2"/>
       <c r="D26" s="2"/>
       <c r="E26" s="2"/>
     </row>
-    <row r="27" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="27" spans="1:5" ht="58" x14ac:dyDescent="0.35">
       <c r="A27" s="4">
         <v>26</v>
       </c>
       <c r="B27" s="2" t="s">
-        <v>19</v>
+        <v>22</v>
       </c>
       <c r="C27" s="2"/>
       <c r="D27" s="2"/>
       <c r="E27" s="2"/>
     </row>
-    <row r="28" spans="1:5" ht="29" x14ac:dyDescent="0.35">
+    <row r="28" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A28" s="4">
         <v>27</v>
       </c>
       <c r="B28" s="2" t="s">
-        <v>55</v>
+        <v>26</v>
       </c>
       <c r="C28" s="2"/>
       <c r="D28" s="2"/>
       <c r="E28" s="2"/>
     </row>
-    <row r="29" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="29" spans="1:5" ht="29" x14ac:dyDescent="0.35">
       <c r="A29" s="4">
         <v>28</v>
       </c>
       <c r="B29" s="2" t="s">
-        <v>56</v>
+        <v>32</v>
       </c>
       <c r="C29" s="2"/>
       <c r="D29" s="2"/>
@@ -997,16 +1008,20 @@
       <c r="A30" s="4">
         <v>29</v>
       </c>
-      <c r="B30" s="2"/>
+      <c r="B30" s="2" t="s">
+        <v>16</v>
+      </c>
       <c r="C30" s="2"/>
       <c r="D30" s="2"/>
       <c r="E30" s="2"/>
     </row>
-    <row r="31" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="31" spans="1:5" ht="29" x14ac:dyDescent="0.35">
       <c r="A31" s="4">
         <v>30</v>
       </c>
-      <c r="B31" s="2"/>
+      <c r="B31" s="2" t="s">
+        <v>27</v>
+      </c>
       <c r="C31" s="2"/>
       <c r="D31" s="2"/>
       <c r="E31" s="2"/>
@@ -1015,7 +1030,9 @@
       <c r="A32" s="4">
         <v>31</v>
       </c>
-      <c r="B32" s="2"/>
+      <c r="B32" s="2" t="s">
+        <v>28</v>
+      </c>
       <c r="C32" s="2"/>
       <c r="D32" s="2"/>
       <c r="E32" s="2"/>
@@ -1024,7 +1041,9 @@
       <c r="A33" s="4">
         <v>32</v>
       </c>
-      <c r="B33" s="2"/>
+      <c r="B33" s="2" t="s">
+        <v>36</v>
+      </c>
       <c r="C33" s="2"/>
       <c r="D33" s="2"/>
       <c r="E33" s="2"/>
@@ -1033,7 +1052,9 @@
       <c r="A34" s="4">
         <v>33</v>
       </c>
-      <c r="B34" s="2"/>
+      <c r="B34" s="2" t="s">
+        <v>37</v>
+      </c>
       <c r="C34" s="2"/>
       <c r="D34" s="2"/>
       <c r="E34" s="2"/>
@@ -1042,7 +1063,9 @@
       <c r="A35" s="4">
         <v>34</v>
       </c>
-      <c r="B35" s="2"/>
+      <c r="B35" s="2" t="s">
+        <v>38</v>
+      </c>
       <c r="C35" s="2"/>
       <c r="D35" s="2"/>
       <c r="E35" s="2"/>
@@ -1051,16 +1074,20 @@
       <c r="A36" s="4">
         <v>35</v>
       </c>
-      <c r="B36" s="2"/>
+      <c r="B36" s="2" t="s">
+        <v>19</v>
+      </c>
       <c r="C36" s="2"/>
       <c r="D36" s="2"/>
       <c r="E36" s="2"/>
     </row>
-    <row r="37" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="37" spans="1:5" ht="29" x14ac:dyDescent="0.35">
       <c r="A37" s="4">
         <v>36</v>
       </c>
-      <c r="B37" s="2"/>
+      <c r="B37" s="2" t="s">
+        <v>54</v>
+      </c>
       <c r="C37" s="2"/>
       <c r="D37" s="2"/>
       <c r="E37" s="2"/>
@@ -1069,7 +1096,9 @@
       <c r="A38" s="4">
         <v>37</v>
       </c>
-      <c r="B38" s="2"/>
+      <c r="B38" s="2" t="s">
+        <v>55</v>
+      </c>
       <c r="C38" s="2"/>
       <c r="D38" s="2"/>
       <c r="E38" s="2"/>
@@ -1184,22 +1213,26 @@
       <c r="D50" s="2"/>
       <c r="E50" s="2"/>
     </row>
-    <row r="51" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="51" spans="1:5" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A51" s="4">
         <v>50</v>
       </c>
-      <c r="B51" s="2"/>
-      <c r="C51" s="2"/>
-      <c r="D51" s="2"/>
+      <c r="B51" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="C51" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="D51" s="2" t="s">
+        <v>50</v>
+      </c>
       <c r="E51" s="2"/>
     </row>
-    <row r="52" spans="1:5" ht="29" x14ac:dyDescent="0.35">
+    <row r="52" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A52" s="4">
         <v>51</v>
       </c>
-      <c r="B52" s="2" t="s">
-        <v>28</v>
-      </c>
+      <c r="B52" s="2"/>
       <c r="C52" s="2"/>
       <c r="D52" s="2"/>
       <c r="E52" s="2"/>
@@ -1208,7 +1241,9 @@
       <c r="A53" s="4">
         <v>52</v>
       </c>
-      <c r="B53" s="2"/>
+      <c r="B53" s="2" t="s">
+        <v>56</v>
+      </c>
       <c r="C53" s="2"/>
       <c r="D53" s="2"/>
       <c r="E53" s="2"/>
@@ -1217,7 +1252,7 @@
   <hyperlinks>
     <hyperlink ref="C2" r:id="rId1" xr:uid="{BCB2A182-B670-418B-99E0-09A7118C3E4A}"/>
     <hyperlink ref="C5" r:id="rId2" xr:uid="{9AA2BF18-F5AA-42E4-B5EA-240371BBCC34}"/>
-    <hyperlink ref="C15" r:id="rId3" xr:uid="{26F759F8-BC11-420B-9F21-9D0D36433723}"/>
+    <hyperlink ref="C24" r:id="rId3" xr:uid="{26F759F8-BC11-420B-9F21-9D0D36433723}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId4"/>

</xml_diff>

<commit_message>
Week something and summat
</commit_message>
<xml_diff>
--- a/Schedule.xlsx
+++ b/Schedule.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26731"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26827"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/0e0481dd48f7e6bd/Python/52-Weeks-of-Python-and-R-2023/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="268" documentId="11_F25DC773A252ABDACC10487A711C7F6A5BDE58EC" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{3D8AA42A-6F4C-4071-8DAB-BC4E2278B0A8}"/>
+  <xr:revisionPtr revIDLastSave="270" documentId="11_F25DC773A252ABDACC10487A711C7F6A5BDE58EC" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{2E15147A-DE61-431E-80BD-0F7FAB2B6093}"/>
   <bookViews>
     <workbookView xWindow="-28920" yWindow="4095" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="99" uniqueCount="79">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="98" uniqueCount="78">
   <si>
     <t>Week</t>
   </si>
@@ -221,9 +221,6 @@
     <t>Optuna for Hyperparameter Optimisation (Swissgrid Challenge)</t>
   </si>
   <si>
-    <t>"Hot Hand" - is it more probable to lose if you've already won many times in a 50/50 scenario? Simulate and use logic</t>
-  </si>
-  <si>
     <t>LSTM/RNN for Time Series Data (aggregate)</t>
   </si>
   <si>
@@ -266,13 +263,13 @@
     <t>yes</t>
   </si>
   <si>
-    <t>Note: Heatmap mit in Visualisierung reinpacken</t>
-  </si>
-  <si>
     <t>Webscraping Digitec Smartphones</t>
   </si>
   <si>
     <t>Analysing Smartphone Specs and Prices</t>
+  </si>
+  <si>
+    <t>"Hot Hand" - is it more probable to lose if you've already won many times in a 50/50 scenario? Simulate and use logic (Gambler's Fallacy)</t>
   </si>
 </sst>
 </file>
@@ -683,7 +680,7 @@
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A20" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B25" sqref="B25"/>
+      <selection pane="bottomLeft" activeCell="B29" sqref="B29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -712,7 +709,7 @@
         <v>4</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
     </row>
     <row r="2" spans="1:6" ht="58" x14ac:dyDescent="0.35">
@@ -732,7 +729,7 @@
         <v>8</v>
       </c>
       <c r="F2" s="4" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
     </row>
     <row r="3" spans="1:6" ht="43.5" x14ac:dyDescent="0.35">
@@ -750,7 +747,7 @@
         <v>12</v>
       </c>
       <c r="F3" s="4" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
     </row>
     <row r="4" spans="1:6" ht="58" x14ac:dyDescent="0.35">
@@ -768,7 +765,7 @@
         <v>23</v>
       </c>
       <c r="F4" s="4" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
     </row>
     <row r="5" spans="1:6" ht="58" x14ac:dyDescent="0.35">
@@ -786,7 +783,7 @@
       </c>
       <c r="E5" s="2"/>
       <c r="F5" s="4" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
     </row>
     <row r="6" spans="1:6" ht="72.5" x14ac:dyDescent="0.35">
@@ -806,7 +803,7 @@
         <v>27</v>
       </c>
       <c r="F6" s="4" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
     </row>
     <row r="7" spans="1:6" ht="43.5" x14ac:dyDescent="0.35">
@@ -822,7 +819,7 @@
       <c r="D7" s="2"/>
       <c r="E7" s="2"/>
       <c r="F7" s="4" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
     </row>
     <row r="8" spans="1:6" ht="29" x14ac:dyDescent="0.35">
@@ -838,7 +835,7 @@
       <c r="D8" s="2"/>
       <c r="E8" s="2"/>
       <c r="F8" s="4" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
     </row>
     <row r="9" spans="1:6" ht="72.5" x14ac:dyDescent="0.35">
@@ -854,7 +851,7 @@
       </c>
       <c r="E9" s="2"/>
       <c r="F9" s="4" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
     </row>
     <row r="10" spans="1:6" ht="43.5" x14ac:dyDescent="0.35">
@@ -870,7 +867,7 @@
       </c>
       <c r="E10" s="2"/>
       <c r="F10" s="4" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
     </row>
     <row r="11" spans="1:6" ht="29" x14ac:dyDescent="0.35">
@@ -886,7 +883,7 @@
       </c>
       <c r="E11" s="2"/>
       <c r="F11" s="4" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
     </row>
     <row r="12" spans="1:6" ht="43.5" x14ac:dyDescent="0.35">
@@ -902,7 +899,7 @@
       </c>
       <c r="E12" s="2"/>
       <c r="F12" s="4" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
     </row>
     <row r="13" spans="1:6" ht="43.5" x14ac:dyDescent="0.35">
@@ -918,7 +915,7 @@
       </c>
       <c r="E13" s="2"/>
       <c r="F13" s="4" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.35">
@@ -932,7 +929,7 @@
       <c r="D14" s="2"/>
       <c r="E14" s="2"/>
       <c r="F14" s="4" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.35">
@@ -946,7 +943,7 @@
       <c r="D15" s="2"/>
       <c r="E15" s="2"/>
       <c r="F15" s="4" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
     </row>
     <row r="16" spans="1:6" x14ac:dyDescent="0.35">
@@ -960,7 +957,7 @@
       <c r="D16" s="2"/>
       <c r="E16" s="2"/>
       <c r="F16" s="4" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
     </row>
     <row r="17" spans="1:6" x14ac:dyDescent="0.35">
@@ -974,7 +971,7 @@
       <c r="D17" s="2"/>
       <c r="E17" s="2"/>
       <c r="F17" s="4" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
     </row>
     <row r="18" spans="1:6" x14ac:dyDescent="0.35">
@@ -988,7 +985,7 @@
       <c r="D18" s="2"/>
       <c r="E18" s="2"/>
       <c r="F18" s="4" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
     </row>
     <row r="19" spans="1:6" x14ac:dyDescent="0.35">
@@ -1002,7 +999,7 @@
       <c r="D19" s="2"/>
       <c r="E19" s="2"/>
       <c r="F19" s="4" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
     </row>
     <row r="20" spans="1:6" x14ac:dyDescent="0.35">
@@ -1016,7 +1013,7 @@
       <c r="D20" s="2"/>
       <c r="E20" s="2"/>
       <c r="F20" s="4" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
     </row>
     <row r="21" spans="1:6" x14ac:dyDescent="0.35">
@@ -1030,7 +1027,7 @@
       <c r="D21" s="2"/>
       <c r="E21" s="2"/>
       <c r="F21" s="4" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
     </row>
     <row r="22" spans="1:6" x14ac:dyDescent="0.35">
@@ -1044,7 +1041,7 @@
       <c r="D22" s="2"/>
       <c r="E22" s="2"/>
       <c r="F22" s="4" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
     </row>
     <row r="23" spans="1:6" x14ac:dyDescent="0.35">
@@ -1076,7 +1073,7 @@
         <v>24</v>
       </c>
       <c r="B25" s="2" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="C25" s="2"/>
       <c r="D25" s="2"/>
@@ -1088,7 +1085,7 @@
         <v>25</v>
       </c>
       <c r="B26" s="2" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="C26" s="2"/>
       <c r="D26" s="2"/>
@@ -1107,17 +1104,15 @@
       <c r="E27" s="2"/>
       <c r="F27" s="4"/>
     </row>
-    <row r="28" spans="1:6" ht="58" x14ac:dyDescent="0.35">
+    <row r="28" spans="1:6" ht="72.5" x14ac:dyDescent="0.35">
       <c r="A28" s="4">
         <v>27</v>
       </c>
       <c r="B28" s="2" t="s">
-        <v>61</v>
+        <v>77</v>
       </c>
       <c r="C28" s="2"/>
-      <c r="D28" s="2" t="s">
-        <v>76</v>
-      </c>
+      <c r="D28" s="2"/>
       <c r="E28" s="2"/>
       <c r="F28" s="4"/>
     </row>
@@ -1126,7 +1121,7 @@
         <v>28</v>
       </c>
       <c r="B29" s="2" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="C29" s="2"/>
       <c r="D29" s="2"/>
@@ -1138,7 +1133,7 @@
         <v>29</v>
       </c>
       <c r="B30" s="2" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="C30" s="5"/>
       <c r="D30" s="2"/>
@@ -1162,7 +1157,7 @@
         <v>31</v>
       </c>
       <c r="B32" s="2" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="C32" s="2"/>
       <c r="D32" s="2"/>
@@ -1222,7 +1217,7 @@
         <v>36</v>
       </c>
       <c r="B37" s="2" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="C37" s="2"/>
       <c r="D37" s="2"/>
@@ -1258,7 +1253,7 @@
         <v>39</v>
       </c>
       <c r="B40" s="2" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="C40" s="2"/>
       <c r="D40" s="2"/>
@@ -1285,7 +1280,7 @@
         <v>18</v>
       </c>
       <c r="C42" s="5" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="D42" s="2"/>
       <c r="E42" s="2"/>
@@ -1296,7 +1291,7 @@
         <v>42</v>
       </c>
       <c r="B43" s="2" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="C43" s="2"/>
       <c r="D43" s="2"/>
@@ -1308,7 +1303,7 @@
         <v>43</v>
       </c>
       <c r="B44" s="2" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="C44" s="2"/>
       <c r="D44" s="2"/>
@@ -1320,7 +1315,7 @@
         <v>44</v>
       </c>
       <c r="B45" s="2" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="C45" s="2"/>
       <c r="D45" s="2"/>
@@ -1332,7 +1327,7 @@
         <v>45</v>
       </c>
       <c r="B46" s="2" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="C46" s="2"/>
       <c r="D46" s="2"/>
@@ -1344,7 +1339,7 @@
         <v>46</v>
       </c>
       <c r="B47" s="2" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="C47" s="2"/>
       <c r="D47" s="2"/>
@@ -1356,7 +1351,7 @@
         <v>47</v>
       </c>
       <c r="B48" s="2" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="C48" s="2"/>
       <c r="D48" s="2"/>

</xml_diff>